<commit_message>
Auto-committed on 2022/01/10 週一
Former-commit-id: 955c27a9650299b0f4d16eb848f65a308d526fcc
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L5-管理性作業/HlAreaLnYg6Pt.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L5-管理性作業/HlAreaLnYg6Pt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -566,6 +566,15 @@
     <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -577,15 +586,6 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -913,10 +913,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="37"/>
       <c r="C1" s="3" t="s">
         <v>61</v>
       </c>
@@ -928,8 +928,8 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
@@ -941,10 +941,10 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="32" t="s">
         <v>56</v>
       </c>
@@ -956,10 +956,10 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
       <c r="E4" s="9"/>
@@ -967,11 +967,11 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="38" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="34" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="12"/>
@@ -980,10 +980,10 @@
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="3"/>
       <c r="D6" s="12"/>
       <c r="E6" s="9"/>
@@ -991,10 +991,10 @@
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="35"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="3"/>
       <c r="D7" s="12"/>
       <c r="E7" s="9"/>
@@ -1068,7 +1068,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="39">
+      <c r="A11" s="35">
         <f t="shared" ref="A11:A20" si="0">A10+1</f>
         <v>3</v>
       </c>
@@ -1089,7 +1089,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="39">
+      <c r="A12" s="35">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1110,7 +1110,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="39">
+      <c r="A13" s="35">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1131,7 +1131,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="39">
+      <c r="A14" s="35">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1152,7 +1152,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="39">
+      <c r="A15" s="35">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1174,7 +1174,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="39">
+      <c r="A16" s="35">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="39">
+      <c r="A17" s="35">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="F17" s="25"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="39">
+      <c r="A18" s="35">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1234,7 +1234,7 @@
       <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="39">
+      <c r="A19" s="35">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="F19" s="25"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="39">
+      <c r="A20" s="35">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1324,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
@@ -1349,10 +1349,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="33" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>